<commit_message>
upload ndc 2.0 notebook preliminary run version
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/ssp_uganda_transformation_cw_ndc_2.xlsx
+++ b/ssp_modeling/scenario_mapping/ssp_uganda_transformation_cw_ndc_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/sisepuede_modeling/ssp_uganda_data/ssp_modeling/scenario_mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED09807-82B1-B44F-8968-0AF01B4DC669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3585CFD-76B3-5345-A6D3-CE5D0D120EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19260" yWindow="660" windowWidth="18980" windowHeight="20800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1640,7 +1640,7 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2819,7 +2819,9 @@
       <c r="H42" s="16">
         <v>0.25</v>
       </c>
-      <c r="I42" s="23"/>
+      <c r="I42" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:9" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
@@ -3354,7 +3356,9 @@
       <c r="H61" s="19">
         <v>1</v>
       </c>
-      <c r="I61" s="23"/>
+      <c r="I61" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:9" s="4" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">

</xml_diff>